<commit_message>
changed from reading CSV to external database
</commit_message>
<xml_diff>
--- a/database/excel_files/preset_database.xlsx
+++ b/database/excel_files/preset_database.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="plan" sheetId="1" r:id="rId1"/>
@@ -887,7 +887,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -940,9 +940,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1238,8 +1235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1336,14 +1333,14 @@
   <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.7109375" style="17" customWidth="1"/>
-    <col min="3" max="3" width="45" style="17" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="17" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" style="17" customWidth="1"/>
+    <col min="2" max="3" width="44.85546875" style="17" customWidth="1"/>
+    <col min="4" max="4" width="61.5703125" style="17" customWidth="1"/>
     <col min="5" max="5" width="63.5703125" style="17" customWidth="1"/>
     <col min="6" max="16384" width="17.28515625" style="17"/>
   </cols>
@@ -1356,10 +1353,10 @@
         <v>3</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>150</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>149</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>151</v>
@@ -1369,14 +1366,14 @@
       <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
-        <v>1</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="9">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="D2" s="9">
-        <v>1</v>
       </c>
       <c r="E2" s="15" t="s">
         <v>4</v>
@@ -1386,14 +1383,14 @@
       <c r="A3" s="9">
         <v>2</v>
       </c>
-      <c r="B3" s="27">
-        <v>1</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="B3" s="9">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9">
+        <v>2</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>5</v>
-      </c>
-      <c r="D3" s="9">
-        <v>2</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>6</v>
@@ -1403,14 +1400,14 @@
       <c r="A4" s="9">
         <v>3</v>
       </c>
-      <c r="B4" s="27">
-        <v>1</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9">
+        <v>2</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>7</v>
-      </c>
-      <c r="D4" s="9">
-        <v>2</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>8</v>
@@ -1423,11 +1420,11 @@
       <c r="B5" s="9">
         <v>1</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="9">
+        <v>2</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="D5" s="9">
-        <v>2</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>10</v>
@@ -1440,11 +1437,11 @@
       <c r="B6" s="9">
         <v>1</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="9">
+        <v>3</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>11</v>
-      </c>
-      <c r="D6" s="9">
-        <v>3</v>
       </c>
       <c r="E6" s="9"/>
     </row>
@@ -1455,11 +1452,11 @@
       <c r="B7" s="9">
         <v>1</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="9">
+        <v>2</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>71</v>
-      </c>
-      <c r="D7" s="9">
-        <v>2</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>72</v>
@@ -1472,11 +1469,11 @@
       <c r="B8" s="9">
         <v>1</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="18">
+        <v>2</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>79</v>
-      </c>
-      <c r="D8" s="18">
-        <v>2</v>
       </c>
       <c r="E8" s="18" t="s">
         <v>83</v>
@@ -1489,11 +1486,11 @@
       <c r="B9" s="9">
         <v>1</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="18">
+        <v>2</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>73</v>
-      </c>
-      <c r="D9" s="18">
-        <v>2</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>74</v>
@@ -1506,11 +1503,11 @@
       <c r="B10" s="9">
         <v>2</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="18">
+        <v>1</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="D10" s="18">
-        <v>1</v>
       </c>
       <c r="E10" s="16" t="s">
         <v>80</v>
@@ -1523,11 +1520,11 @@
       <c r="B11" s="9">
         <v>2</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="9">
+        <v>2</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="D11" s="9">
-        <v>2</v>
       </c>
       <c r="E11" s="15"/>
     </row>
@@ -1538,11 +1535,11 @@
       <c r="B12" s="9">
         <v>2</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="9">
+        <v>2</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="D12" s="9">
-        <v>2</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>75</v>
@@ -1555,11 +1552,11 @@
       <c r="B13" s="9">
         <v>2</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="9">
+        <v>3</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="D13" s="9">
-        <v>3</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>75</v>
@@ -1572,11 +1569,11 @@
       <c r="B14" s="9">
         <v>2</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="18">
+        <v>2</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="D14" s="18">
-        <v>2</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>81</v>
@@ -1589,11 +1586,11 @@
       <c r="B15" s="9">
         <v>2</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="18">
+        <v>2</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="D15" s="18">
-        <v>2</v>
       </c>
       <c r="E15" s="18" t="s">
         <v>76</v>
@@ -1606,11 +1603,11 @@
       <c r="B16" s="9">
         <v>2</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="18">
+        <v>2</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>18</v>
-      </c>
-      <c r="D16" s="18">
-        <v>2</v>
       </c>
       <c r="E16" s="18"/>
     </row>
@@ -1621,11 +1618,11 @@
       <c r="B17" s="9">
         <v>2</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="18">
+        <v>3</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="D17" s="18">
-        <v>3</v>
       </c>
       <c r="E17" s="18" t="s">
         <v>77</v>
@@ -1638,11 +1635,11 @@
       <c r="B18" s="9">
         <v>2</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="18">
+        <v>3</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="D18" s="18">
-        <v>3</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>82</v>
@@ -1652,14 +1649,14 @@
       <c r="A19" s="9">
         <v>18</v>
       </c>
-      <c r="B19" s="28">
-        <v>3</v>
-      </c>
-      <c r="C19" s="29" t="s">
+      <c r="B19" s="27">
+        <v>3</v>
+      </c>
+      <c r="C19" s="18">
+        <v>1</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="D19" s="18">
-        <v>1</v>
       </c>
       <c r="E19" s="18" t="s">
         <v>4</v>
@@ -1669,14 +1666,14 @@
       <c r="A20" s="9">
         <v>19</v>
       </c>
-      <c r="B20" s="28">
-        <v>3</v>
-      </c>
-      <c r="C20" s="29" t="s">
+      <c r="B20" s="27">
+        <v>3</v>
+      </c>
+      <c r="C20" s="18">
+        <v>1</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="D20" s="18">
-        <v>1</v>
       </c>
       <c r="E20" s="18"/>
     </row>
@@ -1684,14 +1681,14 @@
       <c r="A21" s="9">
         <v>20</v>
       </c>
-      <c r="B21" s="28">
-        <v>3</v>
-      </c>
-      <c r="C21" s="6" t="s">
+      <c r="B21" s="27">
+        <v>3</v>
+      </c>
+      <c r="C21" s="18">
+        <v>1</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="D21" s="18">
-        <v>1</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>78</v>
@@ -1701,14 +1698,14 @@
       <c r="A22" s="9">
         <v>21</v>
       </c>
-      <c r="B22" s="28">
-        <v>3</v>
-      </c>
-      <c r="C22" s="18" t="s">
+      <c r="B22" s="27">
+        <v>3</v>
+      </c>
+      <c r="C22" s="18">
+        <v>2</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="D22" s="18">
-        <v>2</v>
       </c>
       <c r="E22" s="18"/>
     </row>
@@ -1716,14 +1713,14 @@
       <c r="A23" s="9">
         <v>22</v>
       </c>
-      <c r="B23" s="28">
-        <v>3</v>
-      </c>
-      <c r="C23" s="18" t="s">
+      <c r="B23" s="27">
+        <v>3</v>
+      </c>
+      <c r="C23" s="18">
+        <v>2</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="D23" s="18">
-        <v>2</v>
       </c>
       <c r="E23" s="18"/>
     </row>
@@ -1731,14 +1728,14 @@
       <c r="A24" s="9">
         <v>23</v>
       </c>
-      <c r="B24" s="28">
-        <v>3</v>
-      </c>
-      <c r="C24" s="29" t="s">
+      <c r="B24" s="27">
+        <v>3</v>
+      </c>
+      <c r="C24" s="18">
+        <v>2</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="D24" s="18">
-        <v>2</v>
       </c>
       <c r="E24" s="18"/>
     </row>
@@ -1746,14 +1743,14 @@
       <c r="A25" s="9">
         <v>24</v>
       </c>
-      <c r="B25" s="28">
-        <v>3</v>
-      </c>
-      <c r="C25" s="18" t="s">
+      <c r="B25" s="27">
+        <v>3</v>
+      </c>
+      <c r="C25" s="18">
+        <v>2</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="D25" s="18">
-        <v>2</v>
       </c>
       <c r="E25" s="18" t="s">
         <v>83</v>
@@ -1763,14 +1760,14 @@
       <c r="A26" s="9">
         <v>25</v>
       </c>
-      <c r="B26" s="28">
-        <v>3</v>
-      </c>
-      <c r="C26" s="18" t="s">
+      <c r="B26" s="27">
+        <v>3</v>
+      </c>
+      <c r="C26" s="18">
+        <v>2</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>65</v>
-      </c>
-      <c r="D26" s="18">
-        <v>2</v>
       </c>
       <c r="E26" s="18"/>
     </row>
@@ -1778,14 +1775,14 @@
       <c r="A27" s="9">
         <v>26</v>
       </c>
-      <c r="B27" s="28">
-        <v>3</v>
-      </c>
-      <c r="C27" s="18" t="s">
+      <c r="B27" s="27">
+        <v>3</v>
+      </c>
+      <c r="C27" s="18">
+        <v>2</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="D27" s="18">
-        <v>2</v>
       </c>
       <c r="E27" s="18" t="s">
         <v>83</v>
@@ -1795,14 +1792,14 @@
       <c r="A28" s="9">
         <v>27</v>
       </c>
-      <c r="B28" s="28">
-        <v>3</v>
-      </c>
-      <c r="C28" s="18" t="s">
+      <c r="B28" s="27">
+        <v>3</v>
+      </c>
+      <c r="C28" s="18">
+        <v>2</v>
+      </c>
+      <c r="D28" s="18" t="s">
         <v>51</v>
-      </c>
-      <c r="D28" s="18">
-        <v>2</v>
       </c>
       <c r="E28" s="18" t="s">
         <v>83</v>
@@ -1812,14 +1809,14 @@
       <c r="A29" s="9">
         <v>28</v>
       </c>
-      <c r="B29" s="28">
-        <v>3</v>
-      </c>
-      <c r="C29" s="29" t="s">
+      <c r="B29" s="27">
+        <v>3</v>
+      </c>
+      <c r="C29" s="18">
+        <v>2</v>
+      </c>
+      <c r="D29" s="28" t="s">
         <v>52</v>
-      </c>
-      <c r="D29" s="18">
-        <v>2</v>
       </c>
       <c r="E29" s="18" t="s">
         <v>83</v>
@@ -1832,11 +1829,11 @@
       <c r="B30" s="9">
         <v>3</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="18">
+        <v>2</v>
+      </c>
+      <c r="D30" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="D30" s="18">
-        <v>2</v>
       </c>
       <c r="E30" s="18" t="s">
         <v>83</v>
@@ -1846,14 +1843,14 @@
       <c r="A31" s="9">
         <v>30</v>
       </c>
-      <c r="B31" s="28">
-        <v>3</v>
-      </c>
-      <c r="C31" s="29" t="s">
+      <c r="B31" s="27">
+        <v>3</v>
+      </c>
+      <c r="C31" s="18">
+        <v>3</v>
+      </c>
+      <c r="D31" s="28" t="s">
         <v>63</v>
-      </c>
-      <c r="D31" s="18">
-        <v>3</v>
       </c>
       <c r="E31" s="18"/>
     </row>
@@ -1861,14 +1858,14 @@
       <c r="A32" s="9">
         <v>31</v>
       </c>
-      <c r="B32" s="28">
-        <v>3</v>
-      </c>
-      <c r="C32" s="18" t="s">
+      <c r="B32" s="27">
+        <v>3</v>
+      </c>
+      <c r="C32" s="18">
+        <v>3</v>
+      </c>
+      <c r="D32" s="18" t="s">
         <v>64</v>
-      </c>
-      <c r="D32" s="18">
-        <v>3</v>
       </c>
       <c r="E32" s="18"/>
     </row>
@@ -1876,14 +1873,14 @@
       <c r="A33" s="9">
         <v>32</v>
       </c>
-      <c r="B33" s="28">
-        <v>3</v>
-      </c>
-      <c r="C33" s="6" t="s">
+      <c r="B33" s="27">
+        <v>3</v>
+      </c>
+      <c r="C33" s="18">
+        <v>3</v>
+      </c>
+      <c r="D33" s="6" t="s">
         <v>11</v>
-      </c>
-      <c r="D33" s="18">
-        <v>3</v>
       </c>
       <c r="E33" s="18"/>
     </row>
@@ -1894,11 +1891,11 @@
       <c r="B34" s="18">
         <v>4</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C34" s="18">
+        <v>3</v>
+      </c>
+      <c r="D34" s="18" t="s">
         <v>105</v>
-      </c>
-      <c r="D34" s="18">
-        <v>3</v>
       </c>
       <c r="E34" s="18"/>
     </row>
@@ -1909,11 +1906,11 @@
       <c r="B35" s="18">
         <v>4</v>
       </c>
-      <c r="C35" s="18" t="s">
+      <c r="C35" s="18">
+        <v>2</v>
+      </c>
+      <c r="D35" s="18" t="s">
         <v>104</v>
-      </c>
-      <c r="D35" s="18">
-        <v>2</v>
       </c>
       <c r="E35" s="18"/>
     </row>
@@ -1924,11 +1921,11 @@
       <c r="B36" s="18">
         <v>4</v>
       </c>
-      <c r="C36" s="29" t="s">
+      <c r="C36" s="18">
+        <v>2</v>
+      </c>
+      <c r="D36" s="28" t="s">
         <v>45</v>
-      </c>
-      <c r="D36" s="18">
-        <v>2</v>
       </c>
       <c r="E36" s="15" t="s">
         <v>4</v>
@@ -1941,11 +1938,11 @@
       <c r="B37" s="18">
         <v>4</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="18">
+        <v>3</v>
+      </c>
+      <c r="D37" s="6" t="s">
         <v>11</v>
-      </c>
-      <c r="D37" s="18">
-        <v>3</v>
       </c>
       <c r="E37" s="18"/>
     </row>
@@ -1956,11 +1953,11 @@
       <c r="B38" s="18">
         <v>4</v>
       </c>
-      <c r="C38" s="23" t="s">
+      <c r="C38" s="18">
+        <v>2</v>
+      </c>
+      <c r="D38" s="23" t="s">
         <v>106</v>
-      </c>
-      <c r="D38" s="18">
-        <v>2</v>
       </c>
       <c r="E38" s="18"/>
     </row>
@@ -1971,11 +1968,11 @@
       <c r="B39" s="18">
         <v>4</v>
       </c>
-      <c r="C39" s="30" t="s">
+      <c r="C39" s="18">
+        <v>2</v>
+      </c>
+      <c r="D39" s="29" t="s">
         <v>107</v>
-      </c>
-      <c r="D39" s="18">
-        <v>2</v>
       </c>
       <c r="E39" s="18" t="s">
         <v>111</v>
@@ -1988,11 +1985,11 @@
       <c r="B40" s="18">
         <v>4</v>
       </c>
-      <c r="C40" s="18" t="s">
+      <c r="C40" s="18">
+        <v>2</v>
+      </c>
+      <c r="D40" s="18" t="s">
         <v>108</v>
-      </c>
-      <c r="D40" s="18">
-        <v>2</v>
       </c>
       <c r="E40" s="18" t="s">
         <v>109</v>
@@ -2005,10 +2002,10 @@
       <c r="B41" s="18">
         <v>4</v>
       </c>
-      <c r="C41" s="30" t="s">
+      <c r="C41" s="18"/>
+      <c r="D41" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="D41" s="18"/>
       <c r="E41" s="18"/>
     </row>
     <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2018,11 +2015,11 @@
       <c r="B42" s="18">
         <v>5</v>
       </c>
-      <c r="C42" s="18" t="s">
+      <c r="C42" s="18">
+        <v>2</v>
+      </c>
+      <c r="D42" s="18" t="s">
         <v>121</v>
-      </c>
-      <c r="D42" s="18">
-        <v>2</v>
       </c>
       <c r="E42" s="18" t="s">
         <v>122</v>
@@ -2035,11 +2032,11 @@
       <c r="B43" s="18">
         <v>5</v>
       </c>
-      <c r="C43" s="18" t="s">
+      <c r="C43" s="18">
+        <v>2</v>
+      </c>
+      <c r="D43" s="18" t="s">
         <v>123</v>
-      </c>
-      <c r="D43" s="18">
-        <v>2</v>
       </c>
       <c r="E43" s="18" t="s">
         <v>124</v>
@@ -2052,11 +2049,11 @@
       <c r="B44" s="18">
         <v>5</v>
       </c>
-      <c r="C44" s="18" t="s">
+      <c r="C44" s="18">
+        <v>2</v>
+      </c>
+      <c r="D44" s="18" t="s">
         <v>125</v>
-      </c>
-      <c r="D44" s="18">
-        <v>2</v>
       </c>
       <c r="E44" s="18" t="s">
         <v>126</v>
@@ -2069,11 +2066,11 @@
       <c r="B45" s="18">
         <v>5</v>
       </c>
-      <c r="C45" s="18" t="s">
+      <c r="C45" s="18">
+        <v>2</v>
+      </c>
+      <c r="D45" s="18" t="s">
         <v>127</v>
-      </c>
-      <c r="D45" s="18">
-        <v>2</v>
       </c>
       <c r="E45" s="18" t="s">
         <v>128</v>
@@ -2086,11 +2083,11 @@
       <c r="B46" s="18">
         <v>5</v>
       </c>
-      <c r="C46" s="18" t="s">
+      <c r="C46" s="18">
+        <v>2</v>
+      </c>
+      <c r="D46" s="18" t="s">
         <v>129</v>
-      </c>
-      <c r="D46" s="18">
-        <v>2</v>
       </c>
       <c r="E46" s="18"/>
     </row>
@@ -2101,11 +2098,11 @@
       <c r="B47" s="18">
         <v>5</v>
       </c>
-      <c r="C47" s="18" t="s">
+      <c r="C47" s="18">
+        <v>2</v>
+      </c>
+      <c r="D47" s="18" t="s">
         <v>130</v>
-      </c>
-      <c r="D47" s="18">
-        <v>2</v>
       </c>
       <c r="E47" s="18" t="s">
         <v>131</v>
@@ -2118,11 +2115,11 @@
       <c r="B48" s="18">
         <v>5</v>
       </c>
-      <c r="C48" s="18" t="s">
+      <c r="C48" s="18">
+        <v>2</v>
+      </c>
+      <c r="D48" s="18" t="s">
         <v>132</v>
-      </c>
-      <c r="D48" s="18">
-        <v>2</v>
       </c>
       <c r="E48" s="18"/>
     </row>
@@ -2133,11 +2130,11 @@
       <c r="B49" s="18">
         <v>5</v>
       </c>
-      <c r="C49" s="18" t="s">
+      <c r="C49" s="18">
+        <v>2</v>
+      </c>
+      <c r="D49" s="18" t="s">
         <v>133</v>
-      </c>
-      <c r="D49" s="18">
-        <v>2</v>
       </c>
       <c r="E49" s="18"/>
     </row>
@@ -2148,11 +2145,11 @@
       <c r="B50" s="18">
         <v>5</v>
       </c>
-      <c r="C50" s="18" t="s">
+      <c r="C50" s="18">
+        <v>2</v>
+      </c>
+      <c r="D50" s="18" t="s">
         <v>134</v>
-      </c>
-      <c r="D50" s="18">
-        <v>2</v>
       </c>
       <c r="E50" s="18" t="s">
         <v>135</v>
@@ -2165,11 +2162,11 @@
       <c r="B51" s="18">
         <v>5</v>
       </c>
-      <c r="C51" s="18" t="s">
+      <c r="C51" s="18">
+        <v>2</v>
+      </c>
+      <c r="D51" s="18" t="s">
         <v>136</v>
-      </c>
-      <c r="D51" s="18">
-        <v>2</v>
       </c>
       <c r="E51" s="18" t="s">
         <v>137</v>
@@ -2182,11 +2179,11 @@
       <c r="B52" s="18">
         <v>5</v>
       </c>
-      <c r="C52" s="18" t="s">
+      <c r="C52" s="18">
+        <v>2</v>
+      </c>
+      <c r="D52" s="18" t="s">
         <v>138</v>
-      </c>
-      <c r="D52" s="18">
-        <v>2</v>
       </c>
       <c r="E52" s="18"/>
     </row>
@@ -2197,11 +2194,11 @@
       <c r="B53" s="18">
         <v>6</v>
       </c>
-      <c r="C53" s="29" t="s">
+      <c r="C53" s="18">
+        <v>1</v>
+      </c>
+      <c r="D53" s="28" t="s">
         <v>45</v>
-      </c>
-      <c r="D53" s="18">
-        <v>1</v>
       </c>
       <c r="E53" s="15" t="s">
         <v>4</v>
@@ -2214,11 +2211,11 @@
       <c r="B54" s="18">
         <v>6</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="C54" s="18">
+        <v>2</v>
+      </c>
+      <c r="D54" s="6" t="s">
         <v>5</v>
-      </c>
-      <c r="D54" s="18">
-        <v>2</v>
       </c>
       <c r="E54" s="9" t="s">
         <v>6</v>
@@ -2231,11 +2228,11 @@
       <c r="B55" s="18">
         <v>6</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="C55" s="18">
+        <v>2</v>
+      </c>
+      <c r="D55" s="6" t="s">
         <v>7</v>
-      </c>
-      <c r="D55" s="18">
-        <v>2</v>
       </c>
       <c r="E55" s="9" t="s">
         <v>8</v>
@@ -2248,11 +2245,11 @@
       <c r="B56" s="18">
         <v>6</v>
       </c>
-      <c r="C56" s="6" t="s">
+      <c r="C56" s="18">
+        <v>1</v>
+      </c>
+      <c r="D56" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="D56" s="18">
-        <v>1</v>
       </c>
       <c r="E56" s="9" t="s">
         <v>10</v>
@@ -2265,11 +2262,11 @@
       <c r="B57" s="18">
         <v>6</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="C57" s="18">
+        <v>2</v>
+      </c>
+      <c r="D57" s="6" t="s">
         <v>71</v>
-      </c>
-      <c r="D57" s="18">
-        <v>2</v>
       </c>
       <c r="E57" s="9" t="s">
         <v>72</v>
@@ -2282,11 +2279,11 @@
       <c r="B58" s="18">
         <v>6</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="C58" s="18">
+        <v>2</v>
+      </c>
+      <c r="D58" s="6" t="s">
         <v>79</v>
-      </c>
-      <c r="D58" s="18">
-        <v>2</v>
       </c>
       <c r="E58" s="18" t="s">
         <v>83</v>
@@ -2299,11 +2296,11 @@
       <c r="B59" s="18">
         <v>6</v>
       </c>
-      <c r="C59" s="6" t="s">
+      <c r="C59" s="18">
+        <v>2</v>
+      </c>
+      <c r="D59" s="6" t="s">
         <v>73</v>
-      </c>
-      <c r="D59" s="18">
-        <v>2</v>
       </c>
       <c r="E59" s="9" t="s">
         <v>74</v>
@@ -2316,13 +2313,13 @@
       <c r="B60" s="18">
         <v>6</v>
       </c>
-      <c r="C60" s="30" t="s">
+      <c r="C60" s="18">
+        <v>2</v>
+      </c>
+      <c r="D60" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="D60" s="18">
-        <v>2</v>
-      </c>
-      <c r="E60" s="31" t="s">
+      <c r="E60" s="30" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2333,11 +2330,11 @@
       <c r="B61" s="18">
         <v>6</v>
       </c>
-      <c r="C61" s="18" t="s">
+      <c r="C61" s="18">
+        <v>2</v>
+      </c>
+      <c r="D61" s="18" t="s">
         <v>18</v>
-      </c>
-      <c r="D61" s="18">
-        <v>2</v>
       </c>
       <c r="E61" s="18"/>
     </row>
@@ -2348,11 +2345,11 @@
       <c r="B62" s="18">
         <v>6</v>
       </c>
-      <c r="C62" s="6" t="s">
+      <c r="C62" s="18">
+        <v>3</v>
+      </c>
+      <c r="D62" s="6" t="s">
         <v>11</v>
-      </c>
-      <c r="D62" s="18">
-        <v>3</v>
       </c>
       <c r="E62" s="18"/>
     </row>
@@ -2363,11 +2360,11 @@
       <c r="B63" s="18">
         <v>6</v>
       </c>
-      <c r="C63" s="18" t="s">
+      <c r="C63" s="18">
+        <v>2</v>
+      </c>
+      <c r="D63" s="18" t="s">
         <v>101</v>
-      </c>
-      <c r="D63" s="18">
-        <v>2</v>
       </c>
       <c r="E63" s="18"/>
     </row>
@@ -2381,7 +2378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>

</xml_diff>